<commit_message>
Fix typo in supply systems database
</commit_message>
<xml_diff>
--- a/cea/databases/CH/assemblies/SUPPLY_NEW.xlsx
+++ b/cea/databases/CH/assemblies/SUPPLY_NEW.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathiasniffeler/Documents/CEA_Testing/ optimisation_test/Test1_SG/inputs/technology/assemblies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nimathia\Documents\CEA_Testing\Keppel_Mediapolis_Biopolis\1stOptimisationTest\inputs\technology\assemblies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CC4DB3-21AC-4541-802F-F1D590AC44EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F3E79FB-5FFB-4F8B-8496-1D26496157B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9360" yWindow="500" windowWidth="29040" windowHeight="15840" tabRatio="993" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9360" yWindow="500" windowWidth="29040" windowHeight="15840" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEATING" sheetId="22" r:id="rId1"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="84">
   <si>
     <t>Description</t>
   </si>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t>secondary_components</t>
-  </si>
-  <si>
-    <t>tertiary_cmponents</t>
   </si>
   <si>
     <t>-</t>
@@ -970,25 +967,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="20.81640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" customWidth="1"/>
+    <col min="11" max="11" width="12.6328125" customWidth="1"/>
+    <col min="13" max="13" width="51.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1002,7 +999,7 @@
         <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>22</v>
@@ -1029,7 +1026,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1037,13 +1034,13 @@
         <v>37</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>3</v>
@@ -1070,7 +1067,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -1078,13 +1075,13 @@
         <v>36</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>6</v>
@@ -1111,7 +1108,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
@@ -1119,13 +1116,13 @@
         <v>38</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>7</v>
@@ -1152,7 +1149,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
@@ -1160,13 +1157,13 @@
         <v>39</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>4</v>
@@ -1193,7 +1190,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
@@ -1201,13 +1198,13 @@
         <v>40</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>5</v>
@@ -1234,7 +1231,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1242,13 +1239,13 @@
         <v>41</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>8</v>
@@ -1275,7 +1272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
@@ -1283,13 +1280,13 @@
         <v>42</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>5</v>
@@ -1316,7 +1313,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
@@ -1324,13 +1321,13 @@
         <v>43</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>5</v>
@@ -1357,7 +1354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1365,13 +1362,13 @@
         <v>44</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>5</v>
@@ -1398,7 +1395,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
@@ -1406,13 +1403,13 @@
         <v>45</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>4</v>
@@ -1439,7 +1436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
@@ -1447,13 +1444,13 @@
         <v>46</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>5</v>
@@ -1480,7 +1477,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
@@ -1488,13 +1485,13 @@
         <v>47</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>5</v>
@@ -1535,20 +1532,20 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" customWidth="1"/>
+    <col min="10" max="10" width="51.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1580,7 +1577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -1612,7 +1609,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>11</v>
       </c>
@@ -1644,7 +1641,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>13</v>
       </c>
@@ -1676,7 +1673,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>14</v>
       </c>
@@ -1708,7 +1705,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
@@ -1740,7 +1737,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
@@ -1772,7 +1769,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>17</v>
       </c>
@@ -1804,7 +1801,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>26</v>
       </c>
@@ -1836,7 +1833,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>18</v>
       </c>
@@ -1868,7 +1865,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
@@ -1900,7 +1897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>28</v>
       </c>
@@ -1932,7 +1929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>29</v>
       </c>
@@ -1974,25 +1971,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="21.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="21.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" customWidth="1"/>
+    <col min="14" max="14" width="51.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2006,7 +2003,7 @@
         <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>68</v>
@@ -2036,7 +2033,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -2044,13 +2041,13 @@
         <v>60</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>3</v>
@@ -2080,7 +2077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>26</v>
       </c>
@@ -2088,13 +2085,13 @@
         <v>61</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>69</v>
@@ -2124,7 +2121,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
@@ -2132,13 +2129,13 @@
         <v>62</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="11" t="s">
         <v>69</v>
@@ -2168,7 +2165,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>30</v>
       </c>
@@ -2176,13 +2173,13 @@
         <v>63</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>69</v>
@@ -2212,7 +2209,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
@@ -2220,13 +2217,13 @@
         <v>64</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F6" s="11" t="s">
         <v>69</v>
@@ -2269,20 +2266,20 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" customWidth="1"/>
+    <col min="10" max="10" width="51.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2314,7 +2311,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
@@ -2346,7 +2343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>20</v>
       </c>

</xml_diff>